<commit_message>
13\01\2023 - full changes
</commit_message>
<xml_diff>
--- a/Trialink/media/results.xlsx
+++ b/Trialink/media/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Position</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Total price</t>
   </si>
   <si>
+    <t xml:space="preserve">Scenario: </t>
+  </si>
+  <si>
     <t>Core Packet: #</t>
   </si>
   <si>
@@ -37,16 +40,16 @@
     <t>EPC 2</t>
   </si>
   <si>
-    <t>licence 150 1</t>
-  </si>
-  <si>
-    <t>licence 150 2</t>
-  </si>
-  <si>
-    <t>iHSS 150</t>
-  </si>
-  <si>
-    <t>iPCRF 150</t>
+    <t>licence 1000 1</t>
+  </si>
+  <si>
+    <t>licence 1000 2</t>
+  </si>
+  <si>
+    <t>iHSS 500</t>
+  </si>
+  <si>
+    <t>iPCRF 500</t>
   </si>
   <si>
     <t>NMS 15endb</t>
@@ -64,88 +67,91 @@
     <t>EPC 50</t>
   </si>
   <si>
-    <t>iHSS 500</t>
-  </si>
-  <si>
     <t>iHSS 50</t>
   </si>
   <si>
-    <t>iPCRF 500</t>
-  </si>
-  <si>
     <t>iPCRF 50</t>
   </si>
   <si>
     <t>Server PoC:</t>
   </si>
   <si>
-    <t>Check Subs qnty</t>
+    <t>RONET Profeccional pack:</t>
+  </si>
+  <si>
+    <t>RONET Professional HW</t>
+  </si>
+  <si>
+    <t>RPV-20000-100 (SW +300 subs)</t>
+  </si>
+  <si>
+    <t>Ronet Professional add licences (+100 subs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional HW+SW equipment: </t>
+  </si>
+  <si>
+    <t>NMS add endB</t>
+  </si>
+  <si>
+    <t>non-Telad eNodeB licence</t>
+  </si>
+  <si>
+    <t>MARS NMS SW 5endB</t>
+  </si>
+  <si>
+    <t>MARS NMS SW 1endB</t>
+  </si>
+  <si>
+    <t>42U</t>
+  </si>
+  <si>
+    <t>SCAT UPS 3000</t>
+  </si>
+  <si>
+    <t>7U box</t>
+  </si>
+  <si>
+    <t>MARS UPS HS-48</t>
+  </si>
+  <si>
+    <t>ESR 21 Router</t>
+  </si>
+  <si>
+    <t>RONET SGW</t>
+  </si>
+  <si>
+    <t>RONET RGW</t>
+  </si>
+  <si>
+    <t>L2 service</t>
+  </si>
+  <si>
+    <t>SFP+10G</t>
+  </si>
+  <si>
+    <t>BTS:</t>
+  </si>
+  <si>
+    <t>eB03H08112</t>
+  </si>
+  <si>
+    <t>Terminals:</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">Additional HW+SW equipment: </t>
-  </si>
-  <si>
-    <t>NMS add endB</t>
-  </si>
-  <si>
-    <t>non-Telad eNodeB licence</t>
-  </si>
-  <si>
-    <t>MARS NMS SW 5endB</t>
-  </si>
-  <si>
-    <t>MARS NMS SW 1endB</t>
-  </si>
-  <si>
-    <t>42U</t>
-  </si>
-  <si>
-    <t>SCAT UPS 3000</t>
-  </si>
-  <si>
-    <t>7U box</t>
-  </si>
-  <si>
-    <t>MARS UPS HS-48</t>
-  </si>
-  <si>
-    <t>ESR 21 Router</t>
-  </si>
-  <si>
-    <t>RONET SGW</t>
-  </si>
-  <si>
-    <t>RONET RGW</t>
-  </si>
-  <si>
-    <t>L2 service</t>
-  </si>
-  <si>
-    <t>SFP+10G</t>
-  </si>
-  <si>
-    <t>BTS:</t>
-  </si>
-  <si>
-    <t>eB03H08112</t>
-  </si>
-  <si>
-    <t>Terminals:</t>
-  </si>
-  <si>
-    <t>P101A</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>Totally for Core packet:</t>
@@ -524,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -551,33 +557,24 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="C2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>24000</v>
-      </c>
-      <c r="E3">
-        <v>24000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -586,15 +583,15 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>24000</v>
+        <v>78400</v>
       </c>
       <c r="E4">
-        <v>24000</v>
+        <v>78400</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -603,15 +600,15 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>39200</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>39200</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -622,13 +619,10 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -637,15 +631,12 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>5400</v>
-      </c>
-      <c r="E7">
-        <v>5400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -654,32 +645,32 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>4640</v>
+        <v>18000</v>
       </c>
       <c r="E8">
-        <v>9280</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>16000</v>
+        <v>7800</v>
       </c>
       <c r="E9">
-        <v>16000</v>
+        <v>31200</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -688,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>3360</v>
+        <v>16000</v>
       </c>
       <c r="E10">
         <v>3360</v>
@@ -696,7 +687,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -705,155 +696,140 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>3840</v>
+        <v>3360</v>
       </c>
       <c r="E11">
-        <v>3840</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>3840</v>
       </c>
       <c r="E12">
-        <v>85880</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>208000</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15">
-        <v>3200</v>
-      </c>
-      <c r="E15">
-        <v>83200</v>
-      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16">
-        <v>1</v>
+      <c r="C16" t="s">
+        <v>43</v>
       </c>
       <c r="D16">
-        <v>18000</v>
+        <v>3200</v>
       </c>
       <c r="E16">
-        <v>18000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17">
         <v>1800</v>
       </c>
       <c r="E17">
-        <v>5400</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C18">
-        <v>2</v>
+      <c r="C18" t="s">
+        <v>43</v>
       </c>
       <c r="D18">
+        <v>780</v>
+      </c>
+      <c r="E18">
         <v>7800</v>
-      </c>
-      <c r="E18">
-        <v>15600</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19">
-        <v>780</v>
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
       </c>
       <c r="E19">
-        <v>4680</v>
+        <v>48800</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20">
-        <v>126880</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="E22">
-        <v>0</v>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -864,423 +840,374 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="D23">
+        <v>4000</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="D24">
+        <v>40000</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>1000</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>54000</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
       </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>1600</v>
-      </c>
-      <c r="E28">
-        <v>3200</v>
-      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
       </c>
       <c r="C29">
-        <v>10</v>
-      </c>
-      <c r="D29">
-        <v>12000</v>
-      </c>
-      <c r="E29">
-        <v>120000</v>
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>2500</v>
+        <v>12000</v>
       </c>
       <c r="E30">
-        <v>2500</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
         <v>27</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>1800</v>
-      </c>
-      <c r="E32">
-        <v>1800</v>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
         <v>29</v>
       </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>2820</v>
-      </c>
-      <c r="E33">
-        <v>2820</v>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>1100</v>
-      </c>
-      <c r="E34">
-        <v>1100</v>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>
       </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>460</v>
-      </c>
-      <c r="E35">
-        <v>460</v>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
       </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>5760</v>
-      </c>
-      <c r="E36">
-        <v>5760</v>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
         <v>33</v>
       </c>
-      <c r="C37">
-        <v>10</v>
-      </c>
-      <c r="D37">
-        <v>9000</v>
-      </c>
-      <c r="E37">
-        <v>90000</v>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
         <v>34</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>5400</v>
-      </c>
-      <c r="E38">
-        <v>5400</v>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
       </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>3500</v>
-      </c>
-      <c r="E39">
-        <v>3500</v>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
       </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>125</v>
-      </c>
-      <c r="E40">
-        <v>125</v>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41">
-        <v>236665</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>0</v>
       </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
       <c r="E42">
-        <v>0</v>
+        <v>50500</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B44" t="s">
         <v>38</v>
       </c>
-      <c r="C44">
-        <v>27</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>27</v>
-      </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>0</v>
       </c>
-      <c r="D45" t="s">
-        <v>48</v>
+      <c r="B45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45">
+        <v>12</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>0</v>
       </c>
+      <c r="D46" t="s">
+        <v>50</v>
+      </c>
       <c r="E46">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>39</v>
-      </c>
-      <c r="E47">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s">
         <v>40</v>
       </c>
-      <c r="C48">
-        <v>788</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>788</v>
-      </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>0</v>
       </c>
-      <c r="D49" t="s">
-        <v>49</v>
-      </c>
-      <c r="E49">
-        <v>788</v>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>0</v>
       </c>
-      <c r="E50">
-        <v>0</v>
+      <c r="D50" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1">
-        <v>1</v>
-      </c>
-      <c r="E51">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1">
         <v>2</v>
       </c>
-      <c r="D54" t="s">
-        <v>50</v>
-      </c>
-      <c r="E54">
-        <v>450240</v>
+      <c r="D55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55">
+        <v>361312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>